<commit_message>
Add StringComparison to column matching
</commit_message>
<xml_diff>
--- a/tests/Resources/RegexMap.xlsx
+++ b/tests/Resources/RegexMap.xlsx
@@ -30,7 +30,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -41,6 +41,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -72,25 +78,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -400,9 +400,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -438,11 +438,11 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
       <c r="A4" s="1">
         <v>5</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="1">
         <v>6</v>
       </c>
       <c r="C4" s="1">

</xml_diff>